<commit_message>
Sửa lỗi cập nhật phân công
</commit_message>
<xml_diff>
--- a/src/main/java/files/DSPhanCong.xlsx
+++ b/src/main/java/files/DSPhanCong.xlsx
@@ -35,16 +35,16 @@
     <t>2023-2024</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
+    <t>Nguyễn Đức Trung</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Phan Văn Anh</t>
   </si>
   <si>
     <t>D21CQCN02-N</t>
-  </si>
-  <si>
-    <t>Trần Minh Hiếu</t>
-  </si>
-  <si>
-    <t>2022-2023</t>
   </si>
 </sst>
 </file>
@@ -114,7 +114,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>1.0</v>
+        <v>1011.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>5</v>
@@ -131,16 +131,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
+        <v>1012.0</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>6</v>
-      </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>1.0</v>
@@ -148,16 +148,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>5.0</v>
+        <v>1013.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n" s="0">
         <v>1.0</v>
@@ -165,19 +165,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>8.0</v>
+        <v>1021.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thêm 1 số thành phần ở view
</commit_message>
<xml_diff>
--- a/src/main/java/files/DSPhanCong.xlsx
+++ b/src/main/java/files/DSPhanCong.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Mã phân công</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>D21CQCN02-N</t>
+  </si>
+  <si>
+    <t>D22CQCN01-N</t>
+  </si>
+  <si>
+    <t>Phạm Bình An</t>
+  </si>
+  <si>
+    <t>Đinh Anh</t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,6 +189,40 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>1026.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>1027.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>